<commit_message>
subbasins data for interpolation
</commit_message>
<xml_diff>
--- a/data/watershed.xlsx
+++ b/data/watershed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\ghnfarid\Projects\meteo-interp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8144B1-CD50-4788-9301-CA32B1BF8F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC816778-BB21-4C6C-BB91-4A9B8AFA3106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,9 +468,21 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4">
+        <v>54</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>

</xml_diff>